<commit_message>
fix bug about ISBN mapping
</commit_message>
<xml_diff>
--- a/doc/colleges.xlsx
+++ b/doc/colleges.xlsx
@@ -252,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,10 +263,12 @@
     <font>
       <sz val="12"/>
       <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -609,25 +611,25 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1">
         <f>ROW(A1)</f>
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>65</v>
@@ -636,16 +638,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <f>ROW(A2)</f>
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>65</v>
@@ -654,17 +656,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <f t="shared" ref="A3:A32" si="0">ROW(A3)</f>
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D3" s="2" t="s">
         <v>64</v>
       </c>
@@ -672,17 +674,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D4" s="2" t="s">
         <v>64</v>
       </c>
@@ -690,17 +692,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D5" s="2" t="s">
         <v>64</v>
       </c>
@@ -708,17 +710,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D6" s="2" t="s">
         <v>64</v>
       </c>
@@ -726,17 +728,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D7" s="2" t="s">
         <v>64</v>
       </c>
@@ -744,17 +746,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D8" s="2" t="s">
         <v>64</v>
       </c>
@@ -762,17 +764,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D9" s="2" t="s">
         <v>64</v>
       </c>
@@ -780,17 +782,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D10" s="2" t="s">
         <v>64</v>
       </c>
@@ -798,17 +800,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D11" s="2" t="s">
         <v>64</v>
       </c>
@@ -816,17 +818,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D12" s="2" t="s">
         <v>64</v>
       </c>
@@ -834,17 +836,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
@@ -852,17 +854,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D14" s="2" t="s">
         <v>64</v>
       </c>
@@ -870,17 +872,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D15" s="2" t="s">
         <v>64</v>
       </c>
@@ -888,17 +890,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="D16" s="2" t="s">
         <v>64</v>
       </c>
@@ -906,17 +908,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="D17" s="2" t="s">
         <v>64</v>
       </c>
@@ -924,17 +926,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="D18" s="2" t="s">
         <v>64</v>
       </c>
@@ -942,17 +944,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D19" s="2" t="s">
         <v>64</v>
       </c>
@@ -960,17 +962,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D20" s="2" t="s">
         <v>64</v>
       </c>
@@ -978,17 +980,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D21" s="2" t="s">
         <v>64</v>
       </c>
@@ -996,17 +998,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D22" s="2" t="s">
         <v>64</v>
       </c>
@@ -1014,17 +1016,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="D23" s="2" t="s">
         <v>64</v>
       </c>
@@ -1032,17 +1034,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="D24" s="2" t="s">
         <v>64</v>
       </c>
@@ -1050,17 +1052,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D25" s="2" t="s">
         <v>64</v>
       </c>
@@ -1068,17 +1070,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D26" s="2" t="s">
         <v>64</v>
       </c>
@@ -1086,17 +1088,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D27" s="2" t="s">
         <v>64</v>
       </c>
@@ -1104,17 +1106,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D28" s="2" t="s">
         <v>64</v>
       </c>
@@ -1122,17 +1124,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D29" s="2" t="s">
         <v>64</v>
       </c>
@@ -1140,17 +1142,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D30" s="2" t="s">
         <v>64</v>
       </c>
@@ -1158,17 +1160,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="D31" s="2" t="s">
         <v>64</v>
       </c>
@@ -1176,16 +1178,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>64</v>

</xml_diff>